<commit_message>
Actualización escaleta tema 01 sexto
Ajustes de escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion01/ESCALETA_MA_06_01_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion01/ESCALETA_MA_06_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="364">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1633,13 +1633,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1655,18 +1667,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6337,8 +6337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E20" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6367,98 +6367,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="33.75" customHeight="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="79" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="79" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="78" t="s">
         <v>275</v>
       </c>
       <c r="F1" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="77" t="s">
         <v>206</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="73" t="s">
         <v>207</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="J1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="73" t="s">
         <v>211</v>
       </c>
-      <c r="L1" s="76" t="s">
+      <c r="L1" s="80" t="s">
         <v>208</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="77" t="s">
+      <c r="N1" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="73" t="s">
+      <c r="O1" s="81"/>
+      <c r="P1" s="72" t="s">
         <v>209</v>
       </c>
-      <c r="Q1" s="79" t="s">
+      <c r="Q1" s="71" t="s">
         <v>210</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="S1" s="82" t="s">
+      <c r="S1" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="T1" s="80" t="s">
+      <c r="T1" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="U1" s="81" t="s">
+      <c r="U1" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="V1" s="80" t="s">
+      <c r="V1" s="74" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A2" s="75"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="74"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="78"/>
       <c r="F2" s="32"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="71"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="73"/>
       <c r="N2" s="30" t="s">
         <v>133</v>
       </c>
       <c r="O2" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="80"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="74"/>
     </row>
     <row r="3" spans="1:24" ht="56">
       <c r="A3" s="33" t="s">
@@ -7184,9 +7184,7 @@
       <c r="D14" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="E14" s="50" t="s">
-        <v>223</v>
-      </c>
+      <c r="E14" s="50"/>
       <c r="F14" s="50"/>
       <c r="G14" s="53" t="s">
         <v>355</v>
@@ -8953,13 +8951,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="P1:P2"/>
@@ -8973,6 +8964,13 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A12 A14:A32">

</xml_diff>